<commit_message>
add strip() to avoid repeated whitespace in final/daily sequence.
</commit_message>
<xml_diff>
--- a/data/Data Description.xlsx
+++ b/data/Data Description.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liutianci/Desktop/research notes/emr/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liutianci/dev/emr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602DA7F0-D802-904A-83E5-3F6547FE4D05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBF2042-BC3E-2742-B1AC-B0A303B241F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="892" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="892" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEMBER" sheetId="2" r:id="rId1"/>
@@ -89,9 +89,9 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Kenneth Moore - Personal View" guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" mergeInterval="0" personalView="1" xWindow="7" yWindow="27" windowWidth="1252" windowHeight="712" tabRatio="964" activeSheetId="1"/>
+    <customWorkbookView name="Jamie Schaeffer - Personal View" guid="{2781825A-5D23-4A4C-A7D6-91EC6A3B8336}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="509" tabRatio="964" activeSheetId="3"/>
     <customWorkbookView name="Kenneth R. Moore - Personal View" guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1268" windowHeight="761" tabRatio="964" activeSheetId="1"/>
-    <customWorkbookView name="Jamie Schaeffer - Personal View" guid="{2781825A-5D23-4A4C-A7D6-91EC6A3B8336}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1020" windowHeight="509" tabRatio="964" activeSheetId="3"/>
-    <customWorkbookView name="Kenneth Moore - Personal View" guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" mergeInterval="0" personalView="1" xWindow="7" yWindow="27" windowWidth="1252" windowHeight="712" tabRatio="964" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1321,14 +1321,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="8">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="181" formatCode="#,##0.0"/>
-    <numFmt numFmtId="182" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -1498,7 +1498,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1513,7 +1513,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1526,7 +1526,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1538,7 +1538,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1880,10 +1880,10 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
@@ -3236,7 +3236,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="356">
+  <cellXfs count="359">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3283,7 +3283,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3295,7 +3295,7 @@
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3322,7 +3322,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3346,7 +3346,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3488,16 +3488,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3541,7 +3541,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="34" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="34" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3586,7 +3586,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3625,13 +3625,13 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3650,7 +3650,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3775,7 +3775,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3832,7 +3832,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3921,7 +3921,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4045,7 +4045,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4104,54 +4104,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4253,17 +4205,78 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1148">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Comma 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
     <cellStyle name="Currency 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Currency 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Currency 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Hyperlink 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Hyperlink 4" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Hyperlink 5" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="13" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Normal 10 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal 10 2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
@@ -5399,10 +5412,6 @@
     <cellStyle name="Style 2 2 9" xfId="1145" xr:uid="{00000000-0005-0000-0000-000075040000}"/>
     <cellStyle name="Style 2 2 9 2" xfId="1146" xr:uid="{00000000-0005-0000-0000-000076040000}"/>
     <cellStyle name="Style 2 2 9 3" xfId="1147" xr:uid="{00000000-0005-0000-0000-000077040000}"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="8" builtinId="8"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
@@ -5420,7 +5429,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5760,22 +5769,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="308" t="s">
+      <c r="A1" s="340" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="309"/>
-      <c r="C1" s="309"/>
-      <c r="D1" s="309"/>
-      <c r="E1" s="309"/>
-      <c r="F1" s="309"/>
+      <c r="B1" s="341"/>
+      <c r="C1" s="341"/>
+      <c r="D1" s="341"/>
+      <c r="E1" s="341"/>
+      <c r="F1" s="341"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="310"/>
-      <c r="B2" s="311"/>
-      <c r="C2" s="311"/>
-      <c r="D2" s="311"/>
-      <c r="E2" s="311"/>
-      <c r="F2" s="311"/>
+      <c r="A2" s="342"/>
+      <c r="B2" s="343"/>
+      <c r="C2" s="343"/>
+      <c r="D2" s="343"/>
+      <c r="E2" s="343"/>
+      <c r="F2" s="343"/>
     </row>
     <row r="3" spans="1:6" s="17" customFormat="1" ht="14">
       <c r="A3" s="61" t="s">
@@ -6077,7 +6086,7 @@
       </c>
       <c r="F18" s="239"/>
     </row>
-    <row r="19" spans="1:6" ht="14">
+    <row r="19" spans="1:6" ht="15">
       <c r="A19" s="146"/>
       <c r="B19" s="111"/>
       <c r="C19" s="110"/>
@@ -6096,8 +6105,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showGridLines="0" showRuler="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showPageBreaks="1" showGridLines="0" printArea="1" showRuler="0">
+      <selection activeCell="A5" sqref="A5"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -6114,8 +6123,8 @@
         <oddFooter>&amp;C&amp;8&amp;P of &amp;N</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showPageBreaks="1" showGridLines="0" printArea="1" showRuler="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showGridLines="0" showRuler="0">
+      <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -6148,10 +6157,12 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <sheetPr codeName="Sheet5"/>
+  <sheetPr codeName="Sheet5">
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="144" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -6166,14 +6177,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="16">
-      <c r="A1" s="306" t="s">
+      <c r="A1" s="356" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="307"/>
-      <c r="C1" s="307"/>
-      <c r="D1" s="307"/>
-      <c r="E1" s="307"/>
-      <c r="F1" s="312"/>
+      <c r="B1" s="357"/>
+      <c r="C1" s="357"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="358"/>
       <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7">
@@ -6332,7 +6343,7 @@
       </c>
       <c r="F10" s="39"/>
     </row>
-    <row r="11" spans="1:7" ht="42">
+    <row r="11" spans="1:7" ht="56">
       <c r="A11" s="77" t="s">
         <v>59</v>
       </c>
@@ -6390,7 +6401,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="42">
+    <row r="14" spans="1:7" ht="56">
       <c r="A14" s="77" t="s">
         <v>93</v>
       </c>
@@ -6567,8 +6578,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showGridLines="0" showRuler="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showGridLines="0" showRuler="0">
+      <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -6585,8 +6596,8 @@
         <oddFooter>&amp;C&amp;8&amp;P of &amp;N</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showGridLines="0" showRuler="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showGridLines="0" showRuler="0">
+      <selection activeCell="C21" sqref="C21"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -6634,22 +6645,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="316" t="s">
+      <c r="A1" s="352" t="s">
         <v>299</v>
       </c>
-      <c r="B1" s="317"/>
-      <c r="C1" s="317"/>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
+      <c r="B1" s="353"/>
+      <c r="C1" s="353"/>
+      <c r="D1" s="353"/>
+      <c r="E1" s="353"/>
+      <c r="F1" s="353"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="318"/>
-      <c r="B2" s="319"/>
-      <c r="C2" s="319"/>
-      <c r="D2" s="319"/>
-      <c r="E2" s="319"/>
-      <c r="F2" s="319"/>
+      <c r="A2" s="354"/>
+      <c r="B2" s="355"/>
+      <c r="C2" s="355"/>
+      <c r="D2" s="355"/>
+      <c r="E2" s="355"/>
+      <c r="F2" s="355"/>
     </row>
     <row r="3" spans="1:6" ht="14">
       <c r="A3" s="137" t="s">
@@ -6725,7 +6736,7 @@
       </c>
       <c r="F6" s="157"/>
     </row>
-    <row r="7" spans="1:6" ht="56">
+    <row r="7" spans="1:6" ht="70">
       <c r="A7" s="74" t="s">
         <v>301</v>
       </c>
@@ -6821,7 +6832,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="56">
+    <row r="12" spans="1:6" ht="70">
       <c r="A12" s="74" t="s">
         <v>302</v>
       </c>
@@ -6841,7 +6852,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="56">
+    <row r="13" spans="1:6" ht="70">
       <c r="A13" s="74" t="s">
         <v>303</v>
       </c>
@@ -6879,7 +6890,7 @@
       </c>
       <c r="F14" s="36"/>
     </row>
-    <row r="15" spans="1:6" ht="14">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15" s="133" t="s">
         <v>203</v>
       </c>
@@ -6937,22 +6948,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="316" t="s">
+      <c r="A1" s="352" t="s">
         <v>304</v>
       </c>
-      <c r="B1" s="317"/>
-      <c r="C1" s="317"/>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
+      <c r="B1" s="353"/>
+      <c r="C1" s="353"/>
+      <c r="D1" s="353"/>
+      <c r="E1" s="353"/>
+      <c r="F1" s="353"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="318"/>
-      <c r="B2" s="319"/>
-      <c r="C2" s="319"/>
-      <c r="D2" s="319"/>
-      <c r="E2" s="319"/>
-      <c r="F2" s="319"/>
+      <c r="A2" s="354"/>
+      <c r="B2" s="355"/>
+      <c r="C2" s="355"/>
+      <c r="D2" s="355"/>
+      <c r="E2" s="355"/>
+      <c r="F2" s="355"/>
     </row>
     <row r="3" spans="1:6" ht="14">
       <c r="A3" s="137" t="s">
@@ -7064,7 +7075,7 @@
       </c>
       <c r="F8" s="36"/>
     </row>
-    <row r="9" spans="1:6" ht="14">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9" s="133" t="s">
         <v>203</v>
       </c>
@@ -7112,14 +7123,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="308" t="s">
+      <c r="A1" s="340" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="309"/>
-      <c r="C1" s="309"/>
-      <c r="D1" s="309"/>
-      <c r="E1" s="309"/>
-      <c r="F1" s="309"/>
+      <c r="B1" s="341"/>
+      <c r="C1" s="341"/>
+      <c r="D1" s="341"/>
+      <c r="E1" s="341"/>
+      <c r="F1" s="341"/>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1" ht="16">
       <c r="A2" s="62" t="s">
@@ -7153,7 +7164,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="98">
+    <row r="4" spans="1:6" ht="112">
       <c r="A4" s="116" t="s">
         <v>132</v>
       </c>
@@ -7171,7 +7182,7 @@
       </c>
       <c r="F4" s="119"/>
     </row>
-    <row r="5" spans="1:6" ht="98">
+    <row r="5" spans="1:6" ht="112">
       <c r="A5" s="85" t="s">
         <v>133</v>
       </c>
@@ -7189,7 +7200,7 @@
       </c>
       <c r="F5" s="49"/>
     </row>
-    <row r="6" spans="1:6" ht="112">
+    <row r="6" spans="1:6" ht="126">
       <c r="A6" s="74" t="s">
         <v>135</v>
       </c>
@@ -7225,7 +7236,7 @@
       </c>
       <c r="F7" s="49"/>
     </row>
-    <row r="8" spans="1:6" ht="112">
+    <row r="8" spans="1:6" ht="126">
       <c r="A8" s="74" t="s">
         <v>137</v>
       </c>
@@ -7388,14 +7399,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16">
-      <c r="A1" s="316" t="s">
+      <c r="A1" s="352" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="317"/>
-      <c r="C1" s="317"/>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
+      <c r="B1" s="353"/>
+      <c r="C1" s="353"/>
+      <c r="D1" s="353"/>
+      <c r="E1" s="353"/>
+      <c r="F1" s="353"/>
     </row>
     <row r="2" spans="1:7" ht="16">
       <c r="A2" s="62" t="s">
@@ -7489,7 +7500,7 @@
       </c>
       <c r="F6" s="126"/>
     </row>
-    <row r="7" spans="1:7" ht="14">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="74" t="s">
         <v>7</v>
       </c>
@@ -7806,14 +7817,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16">
-      <c r="A1" s="316" t="s">
+      <c r="A1" s="352" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="317"/>
-      <c r="C1" s="317"/>
-      <c r="D1" s="317"/>
-      <c r="E1" s="317"/>
-      <c r="F1" s="317"/>
+      <c r="B1" s="353"/>
+      <c r="C1" s="353"/>
+      <c r="D1" s="353"/>
+      <c r="E1" s="353"/>
+      <c r="F1" s="353"/>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="16">
       <c r="A2" s="62" t="s">
@@ -8079,18 +8090,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18">
-      <c r="A1" s="304" t="s">
+      <c r="A1" s="344" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="304"/>
-      <c r="C1" s="304"/>
+      <c r="B1" s="344"/>
+      <c r="C1" s="344"/>
     </row>
     <row r="2" spans="1:3" ht="16">
-      <c r="A2" s="305" t="s">
+      <c r="A2" s="345" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="305"/>
-      <c r="C2" s="305"/>
+      <c r="B2" s="345"/>
+      <c r="C2" s="345"/>
     </row>
     <row r="3" spans="1:3" ht="16">
       <c r="A3" s="51" t="s">
@@ -8110,11 +8121,11 @@
       <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:3" ht="16">
-      <c r="A7" s="306" t="s">
+      <c r="A7" s="346" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="307"/>
-      <c r="C7" s="307"/>
+      <c r="B7" s="347"/>
+      <c r="C7" s="347"/>
     </row>
     <row r="8" spans="1:3" ht="16">
       <c r="A8" s="79"/>
@@ -8309,8 +8320,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showRuler="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showRuler="0" topLeftCell="A2">
+      <selection activeCell="B30" sqref="B30"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -8327,8 +8338,8 @@
         <oddFooter>&amp;C&amp;8&amp;P of &amp;N</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showRuler="0" topLeftCell="A2">
-      <selection activeCell="B30" sqref="B30"/>
+    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showRuler="0">
+      <selection activeCell="B29" sqref="B29"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -8371,14 +8382,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1" ht="16">
-      <c r="B1" s="313" t="s">
+      <c r="B1" s="348" t="s">
         <v>363</v>
       </c>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="315"/>
+      <c r="C1" s="349"/>
+      <c r="D1" s="349"/>
+      <c r="E1" s="349"/>
+      <c r="F1" s="349"/>
+      <c r="G1" s="350"/>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1">
       <c r="B2" s="179"/>
@@ -8429,7 +8440,7 @@
       </c>
       <c r="G4" s="260"/>
     </row>
-    <row r="5" spans="1:7" s="18" customFormat="1" ht="98">
+    <row r="5" spans="1:7" s="18" customFormat="1" ht="112">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -8670,13 +8681,13 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="344"/>
+    <col min="1" max="1" width="10.83203125" style="328"/>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.83203125" style="1" customWidth="1"/>
     <col min="4" max="5" width="10.6640625" customWidth="1"/>
@@ -8686,14 +8697,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16">
-      <c r="B1" s="306" t="s">
+      <c r="B1" s="346" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="307"/>
-      <c r="D1" s="307"/>
-      <c r="E1" s="307"/>
-      <c r="F1" s="307"/>
-      <c r="G1" s="312"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="351"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="59"/>
@@ -8724,8 +8735,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="322" customFormat="1" ht="56">
-      <c r="A4" s="343">
+    <row r="4" spans="1:7" s="306" customFormat="1" ht="56">
+      <c r="A4" s="327">
         <v>1</v>
       </c>
       <c r="B4" s="256" t="s">
@@ -8734,25 +8745,25 @@
       <c r="C4" s="257" t="s">
         <v>157</v>
       </c>
-      <c r="D4" s="330" t="s">
+      <c r="D4" s="314" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="330">
+      <c r="E4" s="314">
         <v>8</v>
       </c>
-      <c r="F4" s="331">
+      <c r="F4" s="315">
         <v>19</v>
       </c>
-      <c r="G4" s="332"/>
-    </row>
-    <row r="5" spans="1:7" s="342" customFormat="1" ht="98">
-      <c r="A5" s="346">
+      <c r="G4" s="316"/>
+    </row>
+    <row r="5" spans="1:7" s="326" customFormat="1" ht="98">
+      <c r="A5" s="330">
         <v>2</v>
       </c>
       <c r="B5" s="74" t="s">
         <v>202</v>
       </c>
-      <c r="C5" s="347" t="s">
+      <c r="C5" s="331" t="s">
         <v>229</v>
       </c>
       <c r="D5" s="70" t="s">
@@ -8761,13 +8772,13 @@
       <c r="E5" s="122">
         <v>8</v>
       </c>
-      <c r="F5" s="348">
+      <c r="F5" s="332">
         <v>19</v>
       </c>
       <c r="G5" s="72"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="42">
-      <c r="A6" s="345">
+      <c r="A6" s="329">
         <v>3</v>
       </c>
       <c r="B6" s="77" t="s">
@@ -8790,7 +8801,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" ht="28">
-      <c r="A7" s="345">
+      <c r="A7" s="329">
         <v>4</v>
       </c>
       <c r="B7" s="77" t="s">
@@ -8810,8 +8821,8 @@
       </c>
       <c r="G7" s="200"/>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="42">
-      <c r="A8" s="345">
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="56">
+      <c r="A8" s="329">
         <v>5</v>
       </c>
       <c r="B8" s="77" t="s">
@@ -8832,7 +8843,7 @@
       <c r="G8" s="200"/>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="56">
-      <c r="A9" s="345">
+      <c r="A9" s="329">
         <v>6</v>
       </c>
       <c r="B9" s="77" t="s">
@@ -8853,7 +8864,7 @@
       <c r="G9" s="200"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="14">
-      <c r="A10" s="345">
+      <c r="A10" s="329">
         <v>7</v>
       </c>
       <c r="B10" s="77" t="s">
@@ -8873,8 +8884,8 @@
       </c>
       <c r="G10" s="200"/>
     </row>
-    <row r="11" spans="1:7" s="322" customFormat="1" ht="56">
-      <c r="A11" s="343">
+    <row r="11" spans="1:7" s="306" customFormat="1" ht="56">
+      <c r="A11" s="327">
         <v>8</v>
       </c>
       <c r="B11" s="276" t="s">
@@ -8883,19 +8894,19 @@
       <c r="C11" s="274" t="s">
         <v>189</v>
       </c>
-      <c r="D11" s="320" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="320">
+      <c r="D11" s="304" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="304">
         <v>19</v>
       </c>
-      <c r="F11" s="321" t="s">
+      <c r="F11" s="305" t="s">
         <v>320</v>
       </c>
       <c r="G11" s="280"/>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="42">
-      <c r="A12" s="345">
+      <c r="A12" s="329">
         <v>9</v>
       </c>
       <c r="B12" s="77" t="s">
@@ -8916,7 +8927,7 @@
       <c r="G12" s="200"/>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="42">
-      <c r="A13" s="345">
+      <c r="A13" s="329">
         <v>10</v>
       </c>
       <c r="B13" s="77" t="s">
@@ -8939,7 +8950,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="14">
-      <c r="A14" s="345">
+      <c r="A14" s="329">
         <v>11</v>
       </c>
       <c r="B14" s="77" t="s">
@@ -8960,7 +8971,7 @@
       <c r="G14" s="200"/>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="42">
-      <c r="A15" s="345">
+      <c r="A15" s="329">
         <v>12</v>
       </c>
       <c r="B15" s="77" t="s">
@@ -8980,8 +8991,8 @@
       </c>
       <c r="G15" s="200"/>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" ht="56">
-      <c r="A16" s="345">
+    <row r="16" spans="1:7" s="7" customFormat="1" ht="70">
+      <c r="A16" s="329">
         <v>13</v>
       </c>
       <c r="B16" s="77" t="s">
@@ -9002,7 +9013,7 @@
       <c r="G16" s="200"/>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" ht="14">
-      <c r="A17" s="345">
+      <c r="A17" s="329">
         <v>14</v>
       </c>
       <c r="B17" s="77" t="s">
@@ -9022,8 +9033,8 @@
       </c>
       <c r="G17" s="200"/>
     </row>
-    <row r="18" spans="1:7" s="322" customFormat="1" ht="14">
-      <c r="A18" s="343">
+    <row r="18" spans="1:7" s="306" customFormat="1" ht="14">
+      <c r="A18" s="327">
         <v>15</v>
       </c>
       <c r="B18" s="273" t="s">
@@ -9032,19 +9043,19 @@
       <c r="C18" s="250" t="s">
         <v>193</v>
       </c>
-      <c r="D18" s="320" t="s">
+      <c r="D18" s="304" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="320">
+      <c r="E18" s="304">
         <v>8</v>
       </c>
-      <c r="F18" s="334" t="s">
+      <c r="F18" s="318" t="s">
         <v>39</v>
       </c>
       <c r="G18" s="280"/>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" ht="28">
-      <c r="A19" s="345">
+      <c r="A19" s="329">
         <v>16</v>
       </c>
       <c r="B19" s="77" t="s">
@@ -9067,7 +9078,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" ht="28">
-      <c r="A20" s="345">
+      <c r="A20" s="329">
         <v>17</v>
       </c>
       <c r="B20" s="77" t="s">
@@ -9090,7 +9101,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="14">
-      <c r="A21" s="345">
+      <c r="A21" s="329">
         <v>18</v>
       </c>
       <c r="B21" s="77" t="s">
@@ -9113,7 +9124,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="14">
-      <c r="A22" s="345">
+      <c r="A22" s="329">
         <v>19</v>
       </c>
       <c r="B22" s="77" t="s">
@@ -9135,14 +9146,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="322" customFormat="1" ht="56">
-      <c r="A23" s="343">
+    <row r="23" spans="1:7" s="306" customFormat="1" ht="56">
+      <c r="A23" s="327">
         <v>20</v>
       </c>
       <c r="B23" s="276" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="333" t="s">
+      <c r="C23" s="317" t="s">
         <v>275</v>
       </c>
       <c r="D23" s="274" t="s">
@@ -9157,7 +9168,7 @@
       <c r="G23" s="280"/>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" ht="28">
-      <c r="A24" s="345">
+      <c r="A24" s="329">
         <v>21</v>
       </c>
       <c r="B24" s="77" t="s">
@@ -9179,14 +9190,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="342" customFormat="1" ht="42">
-      <c r="A25" s="345">
+    <row r="25" spans="1:7" s="326" customFormat="1" ht="42">
+      <c r="A25" s="329">
         <v>22</v>
       </c>
       <c r="B25" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="340" t="s">
+      <c r="C25" s="324" t="s">
         <v>195</v>
       </c>
       <c r="D25" s="73" t="s">
@@ -9198,12 +9209,12 @@
       <c r="F25" s="166" t="s">
         <v>324</v>
       </c>
-      <c r="G25" s="341" t="s">
+      <c r="G25" s="325" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="70">
-      <c r="A26" s="345">
+      <c r="A26" s="329">
         <v>23</v>
       </c>
       <c r="B26" s="77" t="s">
@@ -9224,7 +9235,7 @@
       <c r="G26" s="200"/>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" ht="42">
-      <c r="A27" s="345">
+      <c r="A27" s="329">
         <v>24</v>
       </c>
       <c r="B27" s="77" t="s">
@@ -9245,7 +9256,7 @@
       <c r="G27" s="200"/>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" ht="28">
-      <c r="A28" s="345">
+      <c r="A28" s="329">
         <v>25</v>
       </c>
       <c r="B28" s="77" t="s">
@@ -9267,8 +9278,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="322" customFormat="1" ht="14">
-      <c r="A29" s="343">
+    <row r="29" spans="1:7" s="306" customFormat="1" ht="14">
+      <c r="A29" s="327">
         <v>26</v>
       </c>
       <c r="B29" s="276" t="s">
@@ -9277,19 +9288,19 @@
       <c r="C29" s="250" t="s">
         <v>198</v>
       </c>
-      <c r="D29" s="320" t="s">
+      <c r="D29" s="304" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="320">
+      <c r="E29" s="304">
         <v>8</v>
       </c>
-      <c r="F29" s="334">
+      <c r="F29" s="318">
         <v>12.3</v>
       </c>
       <c r="G29" s="280"/>
     </row>
-    <row r="30" spans="1:7" s="322" customFormat="1" ht="28">
-      <c r="A30" s="343">
+    <row r="30" spans="1:7" s="306" customFormat="1" ht="28">
+      <c r="A30" s="327">
         <v>27</v>
       </c>
       <c r="B30" s="276" t="s">
@@ -9298,19 +9309,19 @@
       <c r="C30" s="250" t="s">
         <v>95</v>
       </c>
-      <c r="D30" s="320" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="320">
+      <c r="D30" s="304" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="304">
         <v>2</v>
       </c>
-      <c r="F30" s="321" t="s">
+      <c r="F30" s="305" t="s">
         <v>323</v>
       </c>
       <c r="G30" s="280"/>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" ht="14">
-      <c r="A31" s="345">
+      <c r="A31" s="329">
         <v>28</v>
       </c>
       <c r="B31" s="77" t="s">
@@ -9333,7 +9344,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" ht="28">
-      <c r="A32" s="345">
+      <c r="A32" s="329">
         <v>29</v>
       </c>
       <c r="B32" s="77" t="s">
@@ -9356,7 +9367,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="28">
-      <c r="A33" s="345">
+      <c r="A33" s="329">
         <v>30</v>
       </c>
       <c r="B33" s="77" t="s">
@@ -9376,8 +9387,8 @@
       </c>
       <c r="G33" s="36"/>
     </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" ht="14">
-      <c r="A34" s="345">
+    <row r="34" spans="1:7" s="1" customFormat="1" ht="28">
+      <c r="A34" s="329">
         <v>31</v>
       </c>
       <c r="B34" s="74" t="s">
@@ -9398,7 +9409,7 @@
       <c r="G34" s="36"/>
     </row>
     <row r="35" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A35" s="345">
+      <c r="A35" s="329">
         <v>32</v>
       </c>
       <c r="B35" s="77" t="s">
@@ -9419,7 +9430,7 @@
       <c r="G35" s="36"/>
     </row>
     <row r="36" spans="1:7" s="18" customFormat="1" ht="14">
-      <c r="A36" s="345">
+      <c r="A36" s="329">
         <v>33</v>
       </c>
       <c r="B36" s="74" t="s">
@@ -9440,7 +9451,7 @@
       <c r="G36" s="36"/>
     </row>
     <row r="37" spans="1:7" ht="14">
-      <c r="A37" s="345">
+      <c r="A37" s="329">
         <v>34</v>
       </c>
       <c r="B37" s="133" t="s">
@@ -9461,7 +9472,7 @@
       <c r="G37" s="229"/>
     </row>
     <row r="38" spans="1:7" s="5" customFormat="1">
-      <c r="A38" s="344"/>
+      <c r="A38" s="328"/>
       <c r="B38" s="147"/>
       <c r="C38" s="148"/>
       <c r="D38" s="147"/>
@@ -9470,7 +9481,7 @@
       <c r="G38" s="106"/>
     </row>
     <row r="39" spans="1:7" s="5" customFormat="1">
-      <c r="A39" s="344"/>
+      <c r="A39" s="328"/>
       <c r="B39" s="147"/>
       <c r="C39" s="148"/>
       <c r="D39" s="147"/>
@@ -9506,8 +9517,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showGridLines="0" showRuler="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showPageBreaks="1" showGridLines="0" printArea="1" showRuler="0">
+      <selection activeCell="F4" sqref="F4"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -9524,8 +9535,8 @@
         <oddFooter>&amp;C&amp;8&amp;P of &amp;N</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showPageBreaks="1" showGridLines="0" printArea="1" showRuler="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showGridLines="0" showRuler="0">
+      <selection activeCell="B23" sqref="B23"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -9558,7 +9569,7 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="211" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="211" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -9572,14 +9583,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1" ht="16">
-      <c r="B1" s="313" t="s">
+      <c r="B1" s="348" t="s">
         <v>371</v>
       </c>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="315"/>
+      <c r="C1" s="349"/>
+      <c r="D1" s="349"/>
+      <c r="E1" s="349"/>
+      <c r="F1" s="349"/>
+      <c r="G1" s="350"/>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1">
       <c r="B2" s="179"/>
@@ -9616,7 +9627,7 @@
       <c r="B4" s="256" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="335" t="s">
+      <c r="C4" s="319" t="s">
         <v>157</v>
       </c>
       <c r="D4" s="258" t="s">
@@ -9630,14 +9641,14 @@
       </c>
       <c r="G4" s="260"/>
     </row>
-    <row r="5" spans="1:7" s="351" customFormat="1" ht="112">
-      <c r="A5" s="351">
+    <row r="5" spans="1:7" s="335" customFormat="1" ht="112">
+      <c r="A5" s="335">
         <v>2</v>
       </c>
       <c r="B5" s="78" t="s">
         <v>202</v>
       </c>
-      <c r="C5" s="352" t="s">
+      <c r="C5" s="336" t="s">
         <v>229</v>
       </c>
       <c r="D5" s="70" t="s">
@@ -9646,7 +9657,7 @@
       <c r="E5" s="70">
         <v>8</v>
       </c>
-      <c r="F5" s="353">
+      <c r="F5" s="337">
         <v>19</v>
       </c>
       <c r="G5" s="72"/>
@@ -9658,7 +9669,7 @@
       <c r="B6" s="273" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="333" t="s">
+      <c r="C6" s="317" t="s">
         <v>179</v>
       </c>
       <c r="D6" s="274" t="s">
@@ -9679,7 +9690,7 @@
       <c r="B7" s="276" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="323" t="s">
+      <c r="C7" s="307" t="s">
         <v>210</v>
       </c>
       <c r="D7" s="274" t="s">
@@ -9691,7 +9702,7 @@
       <c r="F7" s="275" t="s">
         <v>323</v>
       </c>
-      <c r="G7" s="337" t="s">
+      <c r="G7" s="321" t="s">
         <v>209</v>
       </c>
     </row>
@@ -9702,7 +9713,7 @@
       <c r="B8" s="276" t="s">
         <v>368</v>
       </c>
-      <c r="C8" s="323" t="s">
+      <c r="C8" s="307" t="s">
         <v>340</v>
       </c>
       <c r="D8" s="274" t="s">
@@ -9714,7 +9725,7 @@
       <c r="F8" s="275" t="s">
         <v>322</v>
       </c>
-      <c r="G8" s="324" t="s">
+      <c r="G8" s="308" t="s">
         <v>376</v>
       </c>
     </row>
@@ -9725,22 +9736,22 @@
       <c r="B9" s="276" t="s">
         <v>369</v>
       </c>
-      <c r="C9" s="336" t="s">
+      <c r="C9" s="320" t="s">
         <v>366</v>
       </c>
-      <c r="D9" s="338" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="338">
+      <c r="D9" s="322" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="322">
         <v>3</v>
       </c>
       <c r="F9" s="275" t="s">
         <v>332</v>
       </c>
-      <c r="G9" s="339"/>
+      <c r="G9" s="323"/>
     </row>
     <row r="10" spans="1:7" ht="14">
-      <c r="A10" s="351">
+      <c r="A10" s="335">
         <v>7</v>
       </c>
       <c r="B10" s="74" t="s">
@@ -9761,7 +9772,7 @@
       <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:7" ht="14">
-      <c r="A11" s="351">
+      <c r="A11" s="335">
         <v>8</v>
       </c>
       <c r="B11" s="247" t="s">
@@ -9833,7 +9844,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="349"/>
+    <col min="1" max="1" width="9.1640625" style="333"/>
     <col min="2" max="2" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.5" style="6" customWidth="1"/>
     <col min="4" max="5" width="10.6640625" style="5" customWidth="1"/>
@@ -9843,14 +9854,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16">
-      <c r="B1" s="306" t="s">
+      <c r="B1" s="346" t="s">
         <v>256</v>
       </c>
-      <c r="C1" s="307"/>
-      <c r="D1" s="307"/>
-      <c r="E1" s="307"/>
-      <c r="F1" s="307"/>
-      <c r="G1" s="312"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="347"/>
+      <c r="G1" s="351"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="66"/>
@@ -9861,7 +9872,7 @@
       <c r="G2" s="60"/>
     </row>
     <row r="3" spans="1:7" s="17" customFormat="1" ht="14">
-      <c r="A3" s="350"/>
+      <c r="A3" s="334"/>
       <c r="B3" s="61" t="s">
         <v>232</v>
       </c>
@@ -10048,10 +10059,10 @@
       <c r="E11" s="251">
         <v>1</v>
       </c>
-      <c r="F11" s="354" t="s">
+      <c r="F11" s="338" t="s">
         <v>315</v>
       </c>
-      <c r="G11" s="355"/>
+      <c r="G11" s="339"/>
     </row>
     <row r="12" spans="1:7" s="18" customFormat="1" ht="42">
       <c r="A12" s="18">
@@ -10259,7 +10270,7 @@
       <c r="G21" s="108"/>
     </row>
     <row r="22" spans="1:7" s="18" customFormat="1">
-      <c r="A22" s="351"/>
+      <c r="A22" s="335"/>
       <c r="B22" s="115" t="s">
         <v>240</v>
       </c>
@@ -10302,7 +10313,7 @@
   </sheetPr>
   <dimension ref="A1:IV94"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A32" zoomScale="227" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A27" zoomScale="227" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
@@ -10317,14 +10328,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="313" t="s">
+      <c r="A1" s="348" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="315"/>
+      <c r="B1" s="349"/>
+      <c r="C1" s="349"/>
+      <c r="D1" s="349"/>
+      <c r="E1" s="349"/>
+      <c r="F1" s="350"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="179"/>
@@ -10502,7 +10513,7 @@
       </c>
       <c r="F11" s="285"/>
     </row>
-    <row r="12" spans="1:6" ht="28">
+    <row r="12" spans="1:6" ht="42">
       <c r="A12" s="77" t="s">
         <v>205</v>
       </c>
@@ -10594,23 +10605,23 @@
       </c>
       <c r="F16" s="198"/>
     </row>
-    <row r="17" spans="1:256" s="329" customFormat="1" ht="154">
-      <c r="A17" s="325" t="s">
+    <row r="17" spans="1:256" s="313" customFormat="1" ht="154">
+      <c r="A17" s="309" t="s">
         <v>389</v>
       </c>
-      <c r="B17" s="326" t="s">
+      <c r="B17" s="310" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="326" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="326">
+      <c r="C17" s="310" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="310">
         <v>5</v>
       </c>
-      <c r="E17" s="327" t="s">
+      <c r="E17" s="311" t="s">
         <v>316</v>
       </c>
-      <c r="F17" s="328" t="s">
+      <c r="F17" s="312" t="s">
         <v>37</v>
       </c>
     </row>
@@ -13925,8 +13936,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showGridLines="0" showRuler="0" topLeftCell="A25">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showPageBreaks="1" showGridLines="0" printArea="1" showRuler="0">
+      <selection activeCell="G3" sqref="G3"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -13943,8 +13954,8 @@
         <oddFooter>&amp;C&amp;8&amp;P of &amp;N</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{8D848644-9DCD-41A1-9B4A-B4272E5332E0}" showPageBreaks="1" showGridLines="0" printArea="1" showRuler="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <customSheetView guid="{3E74E944-1B7C-4CE4-A7FC-D27C14A12010}" showGridLines="0" showRuler="0" topLeftCell="A25">
+      <selection activeCell="B7" sqref="B7"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0">
@@ -14002,14 +14013,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="308" t="s">
+      <c r="A1" s="340" t="s">
         <v>306</v>
       </c>
-      <c r="B1" s="309"/>
-      <c r="C1" s="309"/>
-      <c r="D1" s="309"/>
-      <c r="E1" s="309"/>
-      <c r="F1" s="309"/>
+      <c r="B1" s="341"/>
+      <c r="C1" s="341"/>
+      <c r="D1" s="341"/>
+      <c r="E1" s="341"/>
+      <c r="F1" s="341"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="154"/>
@@ -14057,7 +14068,7 @@
       </c>
       <c r="F4" s="232"/>
     </row>
-    <row r="5" spans="1:6" customFormat="1" ht="84">
+    <row r="5" spans="1:6" customFormat="1" ht="98">
       <c r="A5" s="76" t="s">
         <v>202</v>
       </c>
@@ -14165,7 +14176,7 @@
       </c>
       <c r="F10" s="39"/>
     </row>
-    <row r="11" spans="1:6" ht="14">
+    <row r="11" spans="1:6" ht="28">
       <c r="A11" s="77" t="s">
         <v>49</v>
       </c>
@@ -14360,8 +14371,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView showGridLines="0" zoomScale="159" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -14375,14 +14386,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="306" t="s">
+      <c r="A1" s="346" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="307"/>
-      <c r="C1" s="307"/>
-      <c r="D1" s="307"/>
-      <c r="E1" s="307"/>
-      <c r="F1" s="312"/>
+      <c r="B1" s="347"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="347"/>
+      <c r="E1" s="347"/>
+      <c r="F1" s="351"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="59"/>
@@ -14520,7 +14531,7 @@
       </c>
       <c r="F9" s="75"/>
     </row>
-    <row r="10" spans="1:6" ht="28">
+    <row r="10" spans="1:6" ht="42">
       <c r="A10" s="74" t="s">
         <v>31</v>
       </c>
@@ -15023,12 +15034,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15261,13 +15267,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931E2005-9AE1-4D2F-AC08-A358D725BF9D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{919208FF-02BC-4E97-80DC-84CF93AF6649}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15293,9 +15304,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{919208FF-02BC-4E97-80DC-84CF93AF6649}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{931E2005-9AE1-4D2F-AC08-A358D725BF9D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>